<commit_message>
working on he lab's lenovo laptop
</commit_message>
<xml_diff>
--- a/output_data/1_auditory_motor.xlsx
+++ b/output_data/1_auditory_motor.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,14 +10,14 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{5CD23671-3BEB-4E1F-B1A8-A327EE96B3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11505" xr2:uid="{516DCEB4-9461-4962-B473-3B3EB4C3ADF7}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>run_num</t>
   </si>
@@ -59,6 +59,87 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>run_num</t>
+  </si>
+  <si>
+    <t>block_num</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>play_duration</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>run_num</t>
+  </si>
+  <si>
+    <t>block_num</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>play_duration</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>run_num</t>
+  </si>
+  <si>
+    <t>block_num</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>play_duration</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -82,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -90,12 +171,18 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,173 +499,181 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1C959E-594C-41EF-81C2-4414377007F5}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="10.85546875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.7109375" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="13.42578125" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="4" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="5.5703125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.25">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0">
+        <v>9.6683938000000005</v>
+      </c>
+      <c r="D2" s="0">
+        <v>999</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.25">
+      <c r="A3" s="0">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C3" s="0">
+        <v>22.919893099999999</v>
+      </c>
+      <c r="D3" s="0">
+        <v>999</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.25">
+      <c r="A4" s="0">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C4" s="0">
+        <v>32.623140999999997</v>
+      </c>
+      <c r="D4" s="0">
+        <v>4.5433914000000044</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
+      <c r="A5" s="0">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>5.8303808999999998</v>
-      </c>
-      <c r="D2">
-        <v>3.3480273</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>19.551525000000002</v>
-      </c>
-      <c r="D3">
-        <v>2.6755958</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>34.9372945</v>
-      </c>
-      <c r="D4">
-        <v>999</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>45.953479799999997</v>
-      </c>
-      <c r="D5">
-        <v>4.2782634000000002</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
+      <c r="C5" s="0">
+        <v>45.600647799999997</v>
+      </c>
+      <c r="D5" s="0">
+        <v>4.823092900000006</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
+      <c r="A6" s="0">
+        <v>0</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
+      <c r="A7" s="0">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
+      <c r="A8" s="0">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
+      <c r="A9" s="0">
+        <v>0</v>
+      </c>
+      <c r="B9" s="0">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chanage no. of blocks, fix image name for end
</commit_message>
<xml_diff>
--- a/output_data/1_auditory_motor.xlsx
+++ b/output_data/1_auditory_motor.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>run_num</t>
   </si>
@@ -134,6 +134,81 @@
   </si>
   <si>
     <t>hand</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>run_num</t>
+  </si>
+  <si>
+    <t>block_num</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>play_duration</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>run_num</t>
+  </si>
+  <si>
+    <t>block_num</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>play_duration</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
   <si>
     <t>L</t>
@@ -163,7 +238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -174,15 +249,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1C959E-594C-41EF-81C2-4414377007F5}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -505,7 +584,7 @@
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="true" customWidth="true"/>
     <col min="2" max="2" width="10.85546875" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.7109375" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" bestFit="true" customWidth="true"/>
     <col min="4" max="4" width="13.42578125" bestFit="true" customWidth="true"/>
     <col min="5" max="5" width="4" bestFit="true" customWidth="true"/>
     <col min="6" max="6" width="5.5703125" bestFit="true" customWidth="true"/>
@@ -513,22 +592,22 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
@@ -539,16 +618,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="0">
-        <v>9.6683938000000005</v>
+        <v>6.1504859999999999</v>
       </c>
       <c r="D2" s="0">
-        <v>999</v>
+        <v>4.1970622999999998</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
@@ -559,16 +638,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="0">
-        <v>22.919893099999999</v>
+        <v>19.272296900000001</v>
       </c>
       <c r="D3" s="0">
-        <v>999</v>
+        <v>4.8683067999999992</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
@@ -579,16 +658,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="0">
-        <v>32.623140999999997</v>
+        <v>33.646056999999999</v>
       </c>
       <c r="D4" s="0">
-        <v>4.5433914000000044</v>
+        <v>4.5297741000000045</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
@@ -599,81 +678,513 @@
         <v>4</v>
       </c>
       <c r="C5" s="0">
-        <v>45.600647799999997</v>
+        <v>45.438324799999997</v>
       </c>
       <c r="D5" s="0">
-        <v>4.823092900000006</v>
+        <v>5.051215500000005</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>58.126281400000003</v>
       </c>
       <c r="D6" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
+        <v>3.9882884999999959</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0">
-        <v>0</v>
+        <v>71.020329399999994</v>
       </c>
       <c r="D7" s="0">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
+        <v>3.579656700000001</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="0">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C8" s="0">
-        <v>0</v>
+        <v>84.358231399999994</v>
       </c>
       <c r="D8" s="0">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
+        <v>3.5401226000000037</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="0">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="0">
-        <v>0</v>
+        <v>97.395813899999993</v>
       </c>
       <c r="D9" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
+        <v>5.1703579000000133</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>1</v>
+      </c>
+      <c r="B10" s="0">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0">
+        <v>110.0291982</v>
+      </c>
+      <c r="D10" s="0">
+        <v>3.1455511000000058</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>1</v>
+      </c>
+      <c r="B11" s="0">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0">
+        <v>123.7041029</v>
+      </c>
+      <c r="D11" s="0">
+        <v>3.4657009000000016</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>1</v>
+      </c>
+      <c r="B12" s="0">
+        <v>11</v>
+      </c>
+      <c r="C12" s="0">
+        <v>136.2573347</v>
+      </c>
+      <c r="D12" s="0">
+        <v>3.8680137000000059</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>1</v>
+      </c>
+      <c r="B13" s="0">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0">
+        <v>149.06848880000001</v>
+      </c>
+      <c r="D13" s="0">
+        <v>3.3220711999999821</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0">
+        <v>161.8688253</v>
+      </c>
+      <c r="D14" s="0">
+        <v>3.7540301999999883</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>1</v>
+      </c>
+      <c r="B15" s="0">
+        <v>14</v>
+      </c>
+      <c r="C15" s="0">
+        <v>174.775172</v>
+      </c>
+      <c r="D15" s="0">
+        <v>3.8532007999999962</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>1</v>
+      </c>
+      <c r="B16" s="0">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0">
+        <v>187.81540029999999</v>
+      </c>
+      <c r="D16" s="0">
+        <v>3.4043962000000079</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>1</v>
+      </c>
+      <c r="B17" s="0">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0">
+        <v>201.20538429999999</v>
+      </c>
+      <c r="D17" s="0">
+        <v>4.0063420000000178</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>0</v>
+      </c>
+      <c r="B18" s="0">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>0</v>
+      </c>
+      <c r="B19" s="0">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>0</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0</v>
+      </c>
+      <c r="C20" s="0">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>0</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0</v>
+      </c>
+      <c r="C21" s="0">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>0</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>0</v>
+      </c>
+      <c r="B23" s="0">
+        <v>0</v>
+      </c>
+      <c r="C23" s="0">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>0</v>
+      </c>
+      <c r="B24" s="0">
+        <v>0</v>
+      </c>
+      <c r="C24" s="0">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>0</v>
+      </c>
+      <c r="B25" s="0">
+        <v>0</v>
+      </c>
+      <c r="C25" s="0">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>0</v>
+      </c>
+      <c r="B26" s="0">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>0</v>
+      </c>
+      <c r="B27" s="0">
+        <v>0</v>
+      </c>
+      <c r="C27" s="0">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>0</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>0</v>
+      </c>
+      <c r="B29" s="0">
+        <v>0</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>0</v>
+      </c>
+      <c r="B30" s="0">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>0</v>
+      </c>
+      <c r="B31" s="0">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>0</v>
+      </c>
+      <c r="B32" s="0">
+        <v>0</v>
+      </c>
+      <c r="C32" s="0">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>0</v>
+      </c>
+      <c r="B33" s="0">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
unify functions into single_run.m + finish roy's review
</commit_message>
<xml_diff>
--- a/output_data/1_auditory_motor.xlsx
+++ b/output_data/1_auditory_motor.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>run_num</t>
   </si>
@@ -215,6 +215,39 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>run_num</t>
+  </si>
+  <si>
+    <t>block_num</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>play_duration</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -238,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -251,17 +284,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +619,7 @@
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="true" customWidth="true"/>
     <col min="2" max="2" width="10.85546875" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.28515625" bestFit="true" customWidth="true"/>
     <col min="4" max="4" width="13.42578125" bestFit="true" customWidth="true"/>
     <col min="5" max="5" width="4" bestFit="true" customWidth="true"/>
     <col min="6" max="6" width="5.5703125" bestFit="true" customWidth="true"/>
@@ -592,22 +627,22 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="0" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
@@ -618,16 +653,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="0">
-        <v>6.1504859999999999</v>
+        <v>999</v>
       </c>
       <c r="D2" s="0">
-        <v>4.1970622999999998</v>
+        <v>999</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
@@ -638,16 +673,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="0">
-        <v>19.272296900000001</v>
+        <v>999</v>
       </c>
       <c r="D3" s="0">
-        <v>4.8683067999999992</v>
+        <v>999</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
@@ -658,16 +693,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="0">
-        <v>33.646056999999999</v>
+        <v>999</v>
       </c>
       <c r="D4" s="0">
-        <v>4.5297741000000045</v>
+        <v>999</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
@@ -678,97 +713,81 @@
         <v>4</v>
       </c>
       <c r="C5" s="0">
-        <v>45.438324799999997</v>
+        <v>999</v>
       </c>
       <c r="D5" s="0">
-        <v>5.051215500000005</v>
+        <v>999</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>58.126281400000003</v>
+        <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>3.9882884999999959</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>53</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0">
-        <v>71.020329399999994</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>3.579656700000001</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>54</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0">
-        <v>84.358231399999994</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>3.5401226000000037</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>54</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0">
-        <v>97.395813899999993</v>
+        <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>5.1703579000000133</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>55</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
     </row>
     <row r="10">
       <c r="A10" s="0">

</xml_diff>

<commit_message>
Finish changes from roy's review
</commit_message>
<xml_diff>
--- a/output_data/1_auditory_motor.xlsx
+++ b/output_data/1_auditory_motor.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t>run_num</t>
   </si>
@@ -215,6 +215,39 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>run_num</t>
+  </si>
+  <si>
+    <t>block_num</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>play_duration</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
   <si>
     <t>run_num</t>
@@ -271,7 +304,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -285,11 +318,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -297,6 +331,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,7 +654,7 @@
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="true" customWidth="true"/>
     <col min="2" max="2" width="10.85546875" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.28515625" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="10.7109375" bestFit="true" customWidth="true"/>
     <col min="4" max="4" width="13.42578125" bestFit="true" customWidth="true"/>
     <col min="5" max="5" width="4" bestFit="true" customWidth="true"/>
     <col min="6" max="6" width="5.5703125" bestFit="true" customWidth="true"/>
@@ -627,22 +662,22 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
@@ -659,10 +694,10 @@
         <v>999</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
@@ -673,16 +708,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="0">
-        <v>999</v>
+        <v>34.082500400000001</v>
       </c>
       <c r="D3" s="0">
-        <v>999</v>
+        <v>1.6276437000000001</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
@@ -693,16 +728,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="0">
-        <v>999</v>
+        <v>49.004559700000001</v>
       </c>
       <c r="D4" s="0">
-        <v>999</v>
+        <v>2.6037429000000003</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
@@ -719,10 +754,10 @@
         <v>999</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Move to interactive structure + other fixes
</commit_message>
<xml_diff>
--- a/output_data/1_auditory_motor.xlsx
+++ b/output_data/1_auditory_motor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\MSc-neuroscience\auditory-experiment-code\output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{018DCA33-FF17-4712-A2CF-C3EED2A09849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC934568-F31A-4259-B2DF-0B5C0917F40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>